<commit_message>
completed the functionality for the whole waiter page
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/WaiterData.xlsx
+++ b/Group14-A2/src/main/java/User/WaiterData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A8F035-6382-4974-AE13-AE97F320FED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464BA2F7-88A5-4EC1-8574-AD2D76DF428B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3396" yWindow="1488" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1896" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="1" r:id="rId1"/>
@@ -59,6 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,19 +408,19 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -470,8 +471,8 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="n">
+        <v>13.0</v>
       </c>
       <c r="H2">
         <v>20</v>

</xml_diff>